<commit_message>
Add Rank 8 for MO and fix typo
</commit_message>
<xml_diff>
--- a/dd5-generator/src/files/MO5.xlsx
+++ b/dd5-generator/src/files/MO5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yann.martin\OneDrive - Doriane sas\Documents\DEV\DD5-Generator\dd5-generator\src\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yann\Documents\DEV\DnD\DD5-Generator\dd5-generator\src\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7341ABD-5983-4BBF-AD6E-4F0FA5A3F3E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC5D8DC-8E8D-4C51-9B54-96948797EE21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12372" yWindow="12948" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="100">
   <si>
     <t>D100</t>
   </si>
@@ -326,6 +326,9 @@
   </si>
   <si>
     <t>Batons magiques (lancer 1d6)</t>
+  </si>
+  <si>
+    <t>Pierres Ioun (lancer 1d4)</t>
   </si>
 </sst>
 </file>
@@ -749,8 +752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -804,7 +807,7 @@
         <v>26</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>27</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1316,7 +1319,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86E3F258-92A1-4454-800C-E125729CDB85}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>